<commit_message>
fixing files, year 2010
</commit_message>
<xml_diff>
--- a/public_html/archivos/2012_1003_OFERTA_ACADEMICA.xlsx
+++ b/public_html/archivos/2012_1003_OFERTA_ACADEMICA.xlsx
@@ -12,38 +12,14 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PREGRADO!$A$5:$L$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">PREGRADO!$A$5:$K$5</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>Flor María Ramón</author>
-  </authors>
-  <commentList>
-    <comment ref="L5" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-En caso que la carrera se encuentre vigente para el segundo ciclo del 2013 seleccione "RATIFICADO" caso contrario"NO VIGENTE HABILITADO". Realizar este proceso solo para las carreras de Estado "VIGENTE" (columna k)</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="100">
   <si>
     <t>CÓDIGO IES</t>
   </si>
@@ -127,9 +103,6 @@
   </si>
   <si>
     <t>SECRETARÍA NACIONAL DE EDUCACIÓN SUPERIOR, CIENCIA, TECNOLOGÍA E INNOVACIÓN</t>
-  </si>
-  <si>
-    <t>RATIFICAR EL ESTADO DE LA CARRERA PARA EL SEGUNDO CICLO DEL 2013 (PRÓXIMO EXAMEN SNNA)</t>
   </si>
   <si>
     <t>NO VIGENTE HABILITADO</t>
@@ -352,7 +325,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -367,12 +340,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -593,10 +560,10 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -691,8 +658,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1933575</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
@@ -1181,10 +1148,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1192,17 +1161,16 @@
     <col min="4" max="4" width="16.7109375" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
     <col min="6" max="7" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="29.7109375" customWidth="1"/>
-    <col min="13" max="13" width="4.5703125" customWidth="1"/>
-    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="12" max="12" width="4.5703125" customWidth="1"/>
+    <col min="13" max="13" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="N1" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M1" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="17" t="s">
         <v>27</v>
       </c>
@@ -1216,14 +1184,13 @@
       <c r="I2" s="17"/>
       <c r="J2" s="17"/>
       <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="N2" s="6" t="s">
+      <c r="M2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
         <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>30</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -1235,10 +1202,9 @@
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-    </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:14" s="5" customFormat="1" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:13" s="5" customFormat="1" ht="64.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1272,22 +1238,19 @@
       <c r="K5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>52</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>11</v>
@@ -1302,27 +1265,27 @@
         <v>24</v>
       </c>
       <c r="I6" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="J6" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="J6" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>56</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>25</v>
@@ -1337,25 +1300,25 @@
         <v>24</v>
       </c>
       <c r="I7" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="11"/>
       <c r="K7" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C8" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>58</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>11</v>
@@ -1370,27 +1333,27 @@
         <v>24</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="11" t="s">
         <v>11</v>
@@ -1405,27 +1368,27 @@
         <v>14</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K9" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C10" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>25</v>
@@ -1440,27 +1403,27 @@
         <v>14</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C11" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="11" t="s">
         <v>62</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="E11" s="11" t="s">
         <v>11</v>
@@ -1475,27 +1438,27 @@
         <v>14</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J11" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K11" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C12" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>11</v>
@@ -1510,33 +1473,33 @@
         <v>24</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B13" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C13" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>13</v>
@@ -1545,24 +1508,24 @@
         <v>14</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J13" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>19</v>
@@ -1580,27 +1543,27 @@
         <v>24</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J14" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="11" t="s">
         <v>67</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>68</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>16</v>
@@ -1615,27 +1578,27 @@
         <v>14</v>
       </c>
       <c r="I15" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K15" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C16" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="8" t="s">
         <v>70</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>71</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>16</v>
@@ -1650,10 +1613,10 @@
         <v>14</v>
       </c>
       <c r="I16" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J16" s="8" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>15</v>
@@ -1661,13 +1624,13 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C17" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D17" s="11" t="s">
         <v>19</v>
@@ -1685,10 +1648,10 @@
         <v>14</v>
       </c>
       <c r="I17" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J17" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K17" s="12" t="s">
         <v>15</v>
@@ -1696,16 +1659,16 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B18" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C18" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>73</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>74</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>11</v>
@@ -1720,10 +1683,10 @@
         <v>24</v>
       </c>
       <c r="I18" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J18" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>20</v>
@@ -1731,22 +1694,22 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B19" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C19" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="D19" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F19" s="11" t="s">
         <v>77</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>78</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>13</v>
@@ -1755,10 +1718,10 @@
         <v>24</v>
       </c>
       <c r="I19" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J19" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K19" s="12" t="s">
         <v>20</v>
@@ -1766,22 +1729,22 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="8" t="s">
-        <v>50</v>
-      </c>
       <c r="C20" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="8" t="s">
         <v>79</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>80</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G20" s="8" t="s">
         <v>13</v>
@@ -1790,10 +1753,10 @@
         <v>14</v>
       </c>
       <c r="I20" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J20" s="8" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K20" s="9" t="s">
         <v>15</v>
@@ -1801,22 +1764,22 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B21" s="11" t="s">
-        <v>50</v>
-      </c>
       <c r="C21" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E21" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G21" s="11" t="s">
         <v>13</v>
@@ -1825,10 +1788,10 @@
         <v>24</v>
       </c>
       <c r="I21" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J21" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="K21" s="12" t="s">
         <v>20</v>
@@ -1836,16 +1799,16 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="B22" s="14" t="s">
-        <v>50</v>
-      </c>
       <c r="C22" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D22" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E22" s="14" t="s">
         <v>16</v>
@@ -1860,32 +1823,28 @@
         <v>24</v>
       </c>
       <c r="I22" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J22" s="14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K22" s="15" t="s">
         <v>20</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A5:L5"/>
+  <autoFilter ref="A5:K5"/>
   <mergeCells count="2">
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="N1:N2 L5">
-      <formula1>$N$1:$N$2</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERROR" error="Solo puede ingresar &quot;RATIFICAR&quot; O &quot;NO VIGENTE HABILITADO&quot;" promptTitle="ERROR" sqref="L6:L22">
-      <formula1>$N$1:$N$2</formula1>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M1:M2">
+      <formula1>$M$1:$M$2</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1929,7 +1888,7 @@
     </row>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="18" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B2" s="18"/>
       <c r="C2" s="18"/>
@@ -1952,10 +1911,10 @@
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>39</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>4</v>
@@ -1973,36 +1932,36 @@
         <v>8</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>10</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="O4" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="C5" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D5" s="16" t="s">
         <v>83</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>84</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>17</v>
@@ -2014,19 +1973,19 @@
         <v>13</v>
       </c>
       <c r="H5" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5" s="16" t="s">
         <v>20</v>
       </c>
       <c r="L5" s="16" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
@@ -2035,40 +1994,40 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B6" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="C6" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D6" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="D6" s="16" t="s">
-        <v>87</v>
-      </c>
       <c r="E6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="G6" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K6" s="16" t="s">
         <v>20</v>
       </c>
       <c r="L6" s="16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
@@ -2077,40 +2036,40 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="C7" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D7" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="D7" s="16" t="s">
-        <v>90</v>
-      </c>
       <c r="E7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="16" t="s">
-        <v>34</v>
-      </c>
       <c r="G7" s="16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I7" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="K7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="L7" s="16" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
@@ -2119,40 +2078,40 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="C8" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="D8" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="D8" s="16" t="s">
-        <v>93</v>
-      </c>
       <c r="E8" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="16" t="s">
         <v>33</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>34</v>
       </c>
       <c r="G8" s="16" t="s">
         <v>13</v>
       </c>
       <c r="H8" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K8" s="16" t="s">
         <v>20</v>
       </c>
       <c r="L8" s="16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
@@ -2161,16 +2120,16 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="16" t="s">
-        <v>50</v>
-      </c>
       <c r="C9" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="D9" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>18</v>
@@ -2182,19 +2141,19 @@
         <v>13</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J9" s="16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K9" s="16" t="s">
         <v>15</v>
       </c>
       <c r="L9" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>

</xml_diff>